<commit_message>
# fix new customer request.
</commit_message>
<xml_diff>
--- a/honeywell/a.projData/List.xlsx
+++ b/honeywell/a.projData/List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="101">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,10 +243,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Testing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>xxpklrp.p</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -284,10 +280,6 @@
   </si>
   <si>
     <t>xxpkltr0.p</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Testing</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -396,6 +388,9 @@
   <si>
     <t>Jordan</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -902,7 +897,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J6" activeCellId="1" sqref="J5 J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -972,7 +967,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>44</v>
@@ -982,10 +977,10 @@
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="1" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1005,17 +1000,17 @@
         <v>2</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H3" s="13">
         <v>41592</v>
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="1" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -1036,15 +1031,15 @@
         <v>2</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="16" t="s">
-        <v>57</v>
+      <c r="J4" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1065,15 +1060,15 @@
         <v>2</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="16" t="s">
-        <v>57</v>
+      <c r="J5" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="K5" s="1"/>
     </row>
@@ -1094,17 +1089,17 @@
         <v>3</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H6" s="19">
         <v>41618</v>
       </c>
       <c r="I6" s="19"/>
-      <c r="J6" s="16" t="s">
-        <v>69</v>
+      <c r="J6" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -1125,10 +1120,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
@@ -1156,10 +1151,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
@@ -1187,10 +1182,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H9" s="13">
         <v>41620</v>
@@ -1220,17 +1215,17 @@
         <v>4</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" s="14">
         <v>41579</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="1" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>47</v>
@@ -1253,7 +1248,7 @@
         <v>3</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="14">
@@ -1284,7 +1279,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1387,327 +1382,327 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="D1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="I1" s="24" t="s">
         <v>76</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F2" s="1">
         <v>22</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F3" s="1">
         <v>23</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F4" s="1">
         <v>24</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F5" s="1">
         <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F6" s="1">
         <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F7" s="1">
         <v>19</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F8" s="1">
         <v>13</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F9" s="1">
         <v>15</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F10" s="1">
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>86</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>88</v>
       </c>
       <c r="F11" s="1">
         <v>16</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F12" s="1">
         <v>5</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I12" s="1"/>
     </row>

</xml_diff>